<commit_message>
further report changes, final tweaks, inclusion of additional graph and unignored the temp files which supposedly aren't temp
</commit_message>
<xml_diff>
--- a/report/results.xlsx
+++ b/report/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATUOS\CSAI\y3\bio\capyle\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2492C331-356E-4877-9D95-A0A2211462EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37BEC4-B479-4915-80AE-5B20D2FF2C3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-15870" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{787A3FB8-3397-480F-ABFF-396DB4DDE3D5}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{787A3FB8-3397-480F-ABFF-396DB4DDE3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="wind gens" sheetId="1" r:id="rId1"/>
     <sheet name="water gens" sheetId="2" r:id="rId2"/>
+    <sheet name="forest fire" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -172,9 +173,6 @@
     <t>10, 182</t>
   </si>
   <si>
-    <t xml:space="preserve">(10,190) (20,200) </t>
-  </si>
-  <si>
     <t>10,190</t>
   </si>
   <si>
@@ -230,13 +228,76 @@
   </si>
   <si>
     <t>140, 150</t>
+  </si>
+  <si>
+    <t>Tests to block bottom of canyon</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>to E</t>
+  </si>
+  <si>
+    <t>to W</t>
+  </si>
+  <si>
+    <t>W + E</t>
+  </si>
+  <si>
+    <t>to N</t>
+  </si>
+  <si>
+    <t>to S</t>
+  </si>
+  <si>
+    <t>at gen 0</t>
+  </si>
+  <si>
+    <t>∞</t>
+  </si>
+  <si>
+    <t>delta gen (0)</t>
+  </si>
+  <si>
+    <t>delta gen (cross)</t>
+  </si>
+  <si>
+    <t>delta gen (cross+10)</t>
+  </si>
+  <si>
+    <t>gen cross</t>
+  </si>
+  <si>
+    <t>gen cross+ 10</t>
+  </si>
+  <si>
+    <t>crossgen</t>
+  </si>
+  <si>
+    <t>x_1, y_1</t>
+  </si>
+  <si>
+    <t>x_2, y_2</t>
+  </si>
+  <si>
+    <t>10,</t>
+  </si>
+  <si>
+    <t>130,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ,200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,13 +325,39 @@
       <name val="DejaVu Sans Mono for Powerline"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -309,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -327,9 +414,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -347,11 +431,188 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="DejaVu Sans Mono for Powerline"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -372,9 +633,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -425,18 +683,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -680,7 +926,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>280</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>349</c:v>
@@ -878,7 +1124,7 @@
                       <c:formatCode>0.00%</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>-6.4285714285714279E-2</c:v>
+                        <c:v>-6.7567567567567988E-3</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>6.8767908309455672E-2</c:v>
@@ -970,7 +1216,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>226.73392857142858</c:v>
+                  <c:v>230.74831081081081</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>264.76719197707735</c:v>
@@ -1089,7 +1335,7 @@
                       <c:formatCode>0.00%</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0.14893617021276595</c:v>
+                        <c:v>0.10030395136778114</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>9.3506493506493538E-2</c:v>
@@ -1184,7 +1430,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.2325227963525835E-2</c:v>
+                  <c:v>4.6773597305512171E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.1137200907974605E-2</c:v>
@@ -1402,6 +1648,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1951295599"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2080,17 +2327,17 @@
     <tableColumn id="1" xr3:uid="{CF9145E6-9A92-4290-A2FE-2216643263E1}" name="Direction"/>
     <tableColumn id="2" xr3:uid="{E2B5D661-5EF5-4A3B-BDBC-AD76A4CE4A9B}" name="Average wind speed (6mgen^-1)"/>
     <tableColumn id="3" xr3:uid="{F5EEB602-1075-4B03-A683-2F4E50D8F512}" name="High Moderate (10mgen^-1)"/>
-    <tableColumn id="8" xr3:uid="{BA2F515F-7772-4893-A81C-2C61EC210934}" name="% Diff" dataDxfId="11" totalsRowDxfId="8">
+    <tableColumn id="8" xr3:uid="{BA2F515F-7772-4893-A81C-2C61EC210934}" name="% Diff" dataDxfId="17" totalsRowDxfId="7">
       <calculatedColumnFormula>1-(1/(Table1[[#This Row],[High Moderate (10mgen^-1)]]/Table1[[#This Row],[Average wind speed (6mgen^-1)]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F32D3504-CFB4-4082-B4FE-033200916E98}" name="Extreme (15mgen^-1)"/>
-    <tableColumn id="9" xr3:uid="{E90D4C9A-5851-4B57-842E-2B8E4B8CDE98}" name="%Diff" dataDxfId="10" totalsRowDxfId="7">
+    <tableColumn id="9" xr3:uid="{E90D4C9A-5851-4B57-842E-2B8E4B8CDE98}" name="%Diff" dataDxfId="16" totalsRowDxfId="6">
       <calculatedColumnFormula>1-(1/(Table1[[#This Row],[Extreme (15mgen^-1)]]/Table1[[#This Row],[High Moderate (10mgen^-1)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0CF70BE5-B268-404C-8064-C33F38D1FA7C}" name="Average generations to reach city" dataDxfId="12" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{0CF70BE5-B268-404C-8064-C33F38D1FA7C}" name="Average generations to reach city" dataDxfId="15" totalsRowDxfId="5">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[Average wind speed (6mgen^-1)]:[Extreme (15mgen^-1)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FFE3271D-1400-4B44-991D-C4182176F045}" name="AVG % Diff" dataDxfId="9" totalsRowDxfId="5">
+    <tableColumn id="10" xr3:uid="{FFE3271D-1400-4B44-991D-C4182176F045}" name="AVG % Diff" dataDxfId="14" totalsRowDxfId="4">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[% Diff]],Table1[[#This Row],[%Diff]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2099,23 +2346,42 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC8920D4-1BBF-4995-B860-FA513B336B74}" name="Table2" displayName="Table2" ref="B2:H25" totalsRowShown="0">
-  <autoFilter ref="B2:H25" xr:uid="{078C8CB9-A90D-4980-A1F3-1D161DC14DFA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G15">
-    <sortCondition ref="E2:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC8920D4-1BBF-4995-B860-FA513B336B74}" name="Table2" displayName="Table2" ref="B2:I26" totalsRowShown="0">
+  <autoFilter ref="B2:I26" xr:uid="{078C8CB9-A90D-4980-A1F3-1D161DC14DFA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I26">
+    <sortCondition descending="1" ref="D2:D26"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5494C4BE-5DF4-4C32-AD6B-49038DFA0521}" name="Top left" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1115D02F-4EF3-4527-BD2A-AEC4186D827A}" name="Bottom right" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E13156E6-4343-4436-BE2B-51C92CFAC8D9}" name="generation square is reached" dataDxfId="1"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5494C4BE-5DF4-4C32-AD6B-49038DFA0521}" name="Top left" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1115D02F-4EF3-4527-BD2A-AEC4186D827A}" name="Bottom right" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{E13156E6-4343-4436-BE2B-51C92CFAC8D9}" name="generation square is reached" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{95D154C6-8267-4230-BC51-86FE585260F4}" name="dump gen"/>
-    <tableColumn id="7" xr3:uid="{5AECB824-B6CE-4AE8-AAA1-DA4530725A7D}" name="gen diff" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{5AECB824-B6CE-4AE8-AAA1-DA4530725A7D}" name="gen diff" dataDxfId="10">
       <calculatedColumnFormula>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{E102F69D-39E0-46EB-8A7B-5770C67B7871}" name="gens to reach"/>
-    <tableColumn id="5" xr3:uid="{6C6D29D6-4A79-42F0-930E-728A5E0D402D}" name="+/-" dataDxfId="2">
-      <calculatedColumnFormula>Table2[[#This Row],[gens to reach]]-$G$3</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{6C6D29D6-4A79-42F0-930E-728A5E0D402D}" name="+/-" dataDxfId="8">
+      <calculatedColumnFormula>Table2[[#This Row],[gens to reach]]-$N$3</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{A14C98A2-243C-4E16-9E4F-59314517CC9A}" name="Reason" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C10BFB8A-15A9-4EF3-BD42-FBDD59C7C3EC}" name="Table3" displayName="Table3" ref="L30:T37" totalsRowShown="0">
+  <autoFilter ref="L30:T37" xr:uid="{D105AECD-B3B2-40F4-8C8E-F87D1A63CA1E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3B673584-FA62-45AF-AA56-783800BDC6B0}" name="x_1, y_1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{33DF2CA5-B5F9-464C-BEBD-5D0EB8422C25}" name="x_2, y_2"/>
+    <tableColumn id="3" xr3:uid="{BCAD9BE5-60CA-4076-8386-63320D31FF7F}" name="crossgen" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6C6C145A-8CAD-4B1C-8F0A-E0DDABF05FA0}" name="at gen 0" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2927CBCD-C3EC-4BB6-9C05-4FA28AE40BBA}" name="gen cross" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{2AD8C1A6-6043-42DB-A619-06C08C087058}" name="gen cross+ 10"/>
+    <tableColumn id="7" xr3:uid="{8B191B06-A60C-4DD4-9704-1CBED8E9746B}" name="delta gen (0)"/>
+    <tableColumn id="8" xr3:uid="{711F246C-9C0E-409B-9610-23BDBBB4CAC4}" name="delta gen (cross)"/>
+    <tableColumn id="9" xr3:uid="{2A1FB801-2725-4A1D-A899-7AEFB7708DE3}" name="delta gen (cross+10)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2421,7 +2687,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:P8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,26 +2787,26 @@
         <v>298</v>
       </c>
       <c r="K3">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="L3" s="7">
         <f>1-(1/(Table1[[#This Row],[High Moderate (10mgen^-1)]]/Table1[[#This Row],[Average wind speed (6mgen^-1)]]))</f>
-        <v>-6.4285714285714279E-2</v>
+        <v>-6.7567567567567988E-3</v>
       </c>
       <c r="M3" s="8">
         <v>329</v>
       </c>
       <c r="N3" s="7">
         <f>1-(1/(Table1[[#This Row],[Extreme (15mgen^-1)]]/Table1[[#This Row],[High Moderate (10mgen^-1)]]))</f>
-        <v>0.14893617021276595</v>
+        <v>0.10030395136778114</v>
       </c>
       <c r="O3" s="6">
         <f>AVERAGE(Table1[[#This Row],[Average wind speed (6mgen^-1)]:[Extreme (15mgen^-1)]])</f>
-        <v>226.73392857142858</v>
+        <v>230.74831081081081</v>
       </c>
       <c r="P3" s="7">
         <f>AVERAGE(Table1[[#This Row],[% Diff]],Table1[[#This Row],[%Diff]])</f>
-        <v>4.2325227963525835E-2</v>
+        <v>4.6773597305512171E-2</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -3002,221 +3268,384 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870154D5-A414-421C-BEDC-FB0A3CC00BBF}">
-  <dimension ref="B2:R25"/>
+  <dimension ref="B2:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="10" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>50</v>
+      <c r="D2" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="S2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="e">
+      <c r="F3" s="29" t="e">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="29">
         <v>306</v>
       </c>
       <c r="H3">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3">
+        <v>306</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="21">
+        <v>172</v>
+      </c>
+      <c r="S3" s="21">
+        <v>182</v>
+      </c>
+      <c r="T3" s="25">
+        <v>10</v>
+      </c>
+      <c r="U3" s="21">
+        <v>298</v>
+      </c>
+      <c r="V3" s="21">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="14">
+        <v>295</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="F4">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="e">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>306</v>
+      </c>
+      <c r="H4">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="Q4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="11">
-        <v>0</v>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>14</v>
+      </c>
+      <c r="T4" s="5">
+        <v>14</v>
+      </c>
+      <c r="U4" s="5">
+        <v>302</v>
+      </c>
+      <c r="V4" s="5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="14">
+        <v>295</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>300</v>
       </c>
       <c r="F5">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="e">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>310</v>
+      </c>
+      <c r="H5">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="21">
+        <v>150</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="25">
+        <v>-150</v>
+      </c>
+      <c r="U5" s="21">
+        <v>303</v>
+      </c>
+      <c r="V5" s="21">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="14">
+        <v>295</v>
       </c>
       <c r="E6">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>14</v>
+        <v>-295</v>
       </c>
       <c r="G6">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="H6">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>-4</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" s="5">
+        <v>77</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <v>-77</v>
+      </c>
+      <c r="U6" s="5">
+        <v>303</v>
+      </c>
+      <c r="V6" s="5">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="14">
+        <v>290</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="F7">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H7">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>20</v>
-      </c>
-      <c r="F8" s="5">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="21">
+        <v>172</v>
+      </c>
+      <c r="S7" s="21">
+        <v>172</v>
+      </c>
+      <c r="T7" s="25">
+        <v>0</v>
+      </c>
+      <c r="U7" s="21">
+        <v>304</v>
+      </c>
+      <c r="V7" s="21">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="31">
+        <v>290</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>20</v>
-      </c>
-      <c r="G8" s="5">
-        <v>312</v>
+        <v>-290</v>
+      </c>
+      <c r="G8" s="28">
+        <v>308</v>
       </c>
       <c r="H8">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="5" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U8" s="5">
+        <v>306</v>
+      </c>
+      <c r="V8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>290</v>
       </c>
       <c r="E9">
@@ -3230,115 +3659,195 @@
         <v>313</v>
       </c>
       <c r="H9">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
         <v>7</v>
       </c>
-      <c r="J9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="15">
-        <v>290</v>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="33">
+        <v>295</v>
+      </c>
+      <c r="S9" s="21">
+        <v>305</v>
+      </c>
+      <c r="T9" s="21">
+        <v>10</v>
+      </c>
+      <c r="U9" s="21">
+        <v>306</v>
+      </c>
+      <c r="V9" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="10">
+        <v>172</v>
       </c>
       <c r="E10">
-        <v>300</v>
-      </c>
-      <c r="F10">
+        <v>182</v>
+      </c>
+      <c r="F10" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
         <v>10</v>
       </c>
       <c r="G10">
+        <v>298</v>
+      </c>
+      <c r="H10">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>-8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="12">
+        <v>80100</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>90110</v>
+      </c>
+      <c r="R10" s="5">
+        <v>157</v>
+      </c>
+      <c r="S10" s="5">
+        <v>167</v>
+      </c>
+      <c r="T10" s="24">
+        <v>10</v>
+      </c>
+      <c r="U10" s="5">
+        <v>306</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="10">
+        <v>172</v>
+      </c>
+      <c r="E11">
+        <v>172</v>
+      </c>
+      <c r="F11" s="16">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>304</v>
+      </c>
+      <c r="H11">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>-2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" s="21">
+        <v>77</v>
+      </c>
+      <c r="S11" s="21">
+        <v>87</v>
+      </c>
+      <c r="T11" s="25">
+        <v>10</v>
+      </c>
+      <c r="U11" s="21">
+        <v>306</v>
+      </c>
+      <c r="V11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="10">
+        <v>172</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>-172</v>
+      </c>
+      <c r="G12">
+        <v>312</v>
+      </c>
+      <c r="H12">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q12" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="31">
+        <v>290</v>
+      </c>
+      <c r="S12" s="5">
+        <v>300</v>
+      </c>
+      <c r="T12" s="5">
+        <v>10</v>
+      </c>
+      <c r="U12" s="5">
         <v>307</v>
       </c>
-      <c r="H10">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="V12" s="5">
         <v>1</v>
       </c>
-      <c r="J10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="15">
-        <v>290</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>-290</v>
-      </c>
-      <c r="G11">
-        <v>308</v>
-      </c>
-      <c r="H11">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>2</v>
-      </c>
-      <c r="J11" t="s">
-        <v>56</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="15">
-        <v>295</v>
-      </c>
-      <c r="E12">
-        <v>300</v>
-      </c>
-      <c r="F12">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>310</v>
-      </c>
-      <c r="H12">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R12" s="9"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="15">
-        <v>295</v>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>80100</v>
+      </c>
+      <c r="C13" s="17">
+        <v>90110</v>
+      </c>
+      <c r="D13" s="10">
+        <v>157</v>
       </c>
       <c r="E13">
-        <v>305</v>
-      </c>
-      <c r="F13">
+        <v>167</v>
+      </c>
+      <c r="F13" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
         <v>10</v>
       </c>
@@ -3346,350 +3855,1028 @@
         <v>306</v>
       </c>
       <c r="H13">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>55</v>
-      </c>
-      <c r="R13" s="9"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="15">
-        <v>295</v>
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R13" s="33">
+        <v>290</v>
+      </c>
+      <c r="S13" s="21">
+        <v>0</v>
+      </c>
+      <c r="T13" s="21">
+        <v>-290</v>
+      </c>
+      <c r="U13" s="21">
+        <v>308</v>
+      </c>
+      <c r="V13" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <v>80100</v>
+      </c>
+      <c r="C14" s="17">
+        <v>90110</v>
+      </c>
+      <c r="D14" s="10">
+        <v>157</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>-295</v>
+        <v>-157</v>
       </c>
       <c r="G14">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H14">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>8</v>
-      </c>
-      <c r="J14" t="s">
-        <v>55</v>
-      </c>
-      <c r="R14" s="9"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="12">
         <v>80100</v>
       </c>
-      <c r="C15" s="18">
+      <c r="Q14" s="23">
         <v>90110</v>
       </c>
-      <c r="D15" s="11">
+      <c r="R14" s="5">
         <v>157</v>
       </c>
+      <c r="S14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>-157</v>
+      </c>
+      <c r="U14" s="5">
+        <v>309</v>
+      </c>
+      <c r="V14" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>80100</v>
+      </c>
+      <c r="C15" s="17">
+        <v>90110</v>
+      </c>
+      <c r="D15" s="10">
+        <v>157</v>
+      </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+        <v>157</v>
+      </c>
+      <c r="F15" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>-157</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>309</v>
       </c>
       <c r="H15">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
         <v>3</v>
       </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="I15" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="20">
+        <v>80100</v>
+      </c>
+      <c r="Q15" s="22">
+        <v>90110</v>
+      </c>
+      <c r="R15" s="21">
+        <v>157</v>
+      </c>
+      <c r="S15" s="21">
+        <v>157</v>
+      </c>
+      <c r="T15" s="25">
+        <v>0</v>
+      </c>
+      <c r="U15" s="21">
+        <v>309</v>
+      </c>
+      <c r="V15" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>150</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
         <v>-150</v>
       </c>
       <c r="G16">
         <v>303</v>
       </c>
-      <c r="H16" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="H16">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
         <v>-3</v>
       </c>
-      <c r="J16" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
-        <v>80100</v>
-      </c>
-      <c r="C17" s="18">
-        <v>90110</v>
-      </c>
-      <c r="D17" s="11">
-        <v>157</v>
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="P16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R16" s="5">
+        <v>150</v>
+      </c>
+      <c r="S16" s="5">
+        <v>160</v>
+      </c>
+      <c r="T16" s="24">
+        <v>10</v>
+      </c>
+      <c r="U16" s="5">
+        <v>309</v>
+      </c>
+      <c r="V16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="10">
+        <v>150</v>
       </c>
       <c r="E17">
-        <v>157</v>
-      </c>
-      <c r="F17" s="17">
+        <v>160</v>
+      </c>
+      <c r="F17" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <v>309</v>
       </c>
-      <c r="H17" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="H17">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
         <v>3</v>
       </c>
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>80100</v>
-      </c>
-      <c r="C18" s="18">
-        <v>90110</v>
-      </c>
-      <c r="D18" s="11">
-        <v>157</v>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17" s="33">
+        <v>295</v>
+      </c>
+      <c r="S17" s="21">
+        <v>300</v>
+      </c>
+      <c r="T17" s="21">
+        <v>5</v>
+      </c>
+      <c r="U17" s="21">
+        <v>310</v>
+      </c>
+      <c r="V17" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="10">
+        <v>150</v>
       </c>
       <c r="E18">
-        <v>167</v>
-      </c>
-      <c r="F18" s="17">
+        <v>150</v>
+      </c>
+      <c r="F18" s="16">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>310</v>
+      </c>
+      <c r="H18">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R18" s="5">
+        <v>150</v>
+      </c>
+      <c r="S18" s="5">
+        <v>150</v>
+      </c>
+      <c r="T18" s="24">
+        <v>0</v>
+      </c>
+      <c r="U18" s="5">
+        <v>310</v>
+      </c>
+      <c r="V18" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="27">
+        <v>77</v>
+      </c>
+      <c r="E19" s="29">
+        <v>0</v>
+      </c>
+      <c r="F19" s="34">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>-77</v>
+      </c>
+      <c r="G19" s="29">
+        <v>303</v>
+      </c>
+      <c r="H19">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>-3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="R19" s="21">
+        <v>77</v>
+      </c>
+      <c r="S19" s="21">
+        <v>77</v>
+      </c>
+      <c r="T19" s="25">
+        <v>0</v>
+      </c>
+      <c r="U19" s="21">
+        <v>311</v>
+      </c>
+      <c r="V19" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="10">
+        <v>77</v>
+      </c>
+      <c r="E20">
+        <v>87</v>
+      </c>
+      <c r="F20" s="16">
         <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
         <v>10</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>306</v>
       </c>
-      <c r="H18" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="H20">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" s="5">
+        <v>0</v>
+      </c>
+      <c r="S20" s="5">
+        <v>15</v>
+      </c>
+      <c r="T20" s="5">
+        <v>15</v>
+      </c>
+      <c r="U20" s="5">
+        <v>312</v>
+      </c>
+      <c r="V20" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="11">
+      <c r="C21" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="10">
+        <v>77</v>
+      </c>
+      <c r="E21">
+        <v>77</v>
+      </c>
+      <c r="F21" s="16">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>311</v>
+      </c>
+      <c r="H21">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="R21" s="21">
+        <v>0</v>
+      </c>
+      <c r="S21" s="21">
+        <v>20</v>
+      </c>
+      <c r="T21" s="21">
+        <v>20</v>
+      </c>
+      <c r="U21" s="21">
+        <v>312</v>
+      </c>
+      <c r="V21" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>302</v>
+      </c>
+      <c r="H22">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>-4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R22" s="5">
+        <v>172</v>
+      </c>
+      <c r="S22" s="5">
+        <v>0</v>
+      </c>
+      <c r="T22" s="24">
+        <v>-172</v>
+      </c>
+      <c r="U22" s="5">
+        <v>312</v>
+      </c>
+      <c r="V22" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>312</v>
+      </c>
+      <c r="H23">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
+      </c>
+      <c r="P23" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q23" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R23" s="33">
+        <v>290</v>
+      </c>
+      <c r="S23" s="21">
+        <v>295</v>
+      </c>
+      <c r="T23" s="21">
+        <v>5</v>
+      </c>
+      <c r="U23" s="21">
+        <v>313</v>
+      </c>
+      <c r="V23" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="27">
+        <v>0</v>
+      </c>
+      <c r="E24" s="27">
+        <v>20</v>
+      </c>
+      <c r="F24" s="27">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>20</v>
+      </c>
+      <c r="G24" s="27">
+        <v>312</v>
+      </c>
+      <c r="H24">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q24" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="R24" s="31">
+        <v>295</v>
+      </c>
+      <c r="S24" s="5">
+        <v>0</v>
+      </c>
+      <c r="T24" s="5">
+        <v>-295</v>
+      </c>
+      <c r="U24" s="5">
+        <v>314</v>
+      </c>
+      <c r="V24" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q25" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="R25" s="21">
+        <v>0</v>
+      </c>
+      <c r="S25" s="21">
+        <v>0</v>
+      </c>
+      <c r="T25" s="21">
+        <v>0</v>
+      </c>
+      <c r="U25" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="V25" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="e">
+        <f>Table2[[#This Row],[gens to reach]]-$N$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R26" s="5">
+        <v>0</v>
+      </c>
+      <c r="S26" s="5">
+        <v>13</v>
+      </c>
+      <c r="T26" s="5">
+        <v>13</v>
+      </c>
+      <c r="U26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V26" s="5" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" t="s">
+        <v>82</v>
+      </c>
+      <c r="N30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O30" t="s">
+        <v>73</v>
+      </c>
+      <c r="P30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>79</v>
+      </c>
+      <c r="R30" t="s">
+        <v>75</v>
+      </c>
+      <c r="S30" t="s">
+        <v>76</v>
+      </c>
+      <c r="T30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L31" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N31" s="31">
+        <v>295</v>
+      </c>
+      <c r="O31" s="5">
+        <v>314</v>
+      </c>
+      <c r="P31" s="21">
+        <v>310</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>306</v>
+      </c>
+      <c r="R31">
+        <f>O31-$N$3</f>
+        <v>8</v>
+      </c>
+      <c r="S31">
+        <f>P31-$N$3</f>
+        <v>4</v>
+      </c>
+      <c r="T31">
+        <f t="shared" ref="S31:T31" si="0">Q31-$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L32" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N32" s="33">
+        <v>290</v>
+      </c>
+      <c r="O32" s="5">
+        <v>308</v>
+      </c>
+      <c r="P32" s="21">
+        <v>313</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>307</v>
+      </c>
+      <c r="R32">
+        <f t="shared" ref="R32:R36" si="1">O32-$N$3</f>
+        <v>2</v>
+      </c>
+      <c r="S32">
+        <f t="shared" ref="S32:S36" si="2">P32-$N$3</f>
+        <v>7</v>
+      </c>
+      <c r="T32">
+        <f t="shared" ref="T32:T36" si="3">Q32-$N$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="L33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="5">
+        <v>172</v>
+      </c>
+      <c r="O33" s="5">
+        <v>312</v>
+      </c>
+      <c r="P33" s="21">
+        <v>304</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>298</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="34" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E34" s="37">
+        <v>10190</v>
+      </c>
+      <c r="L34" s="20">
+        <v>80100</v>
+      </c>
+      <c r="M34" s="22">
+        <v>90110</v>
+      </c>
+      <c r="N34" s="21">
+        <v>157</v>
+      </c>
+      <c r="O34" s="5">
+        <v>309</v>
+      </c>
+      <c r="P34" s="21">
+        <v>309</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>306</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E35" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="L35" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35" s="5">
         <v>150</v>
       </c>
-      <c r="E19">
-        <v>160</v>
-      </c>
-      <c r="F19" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>10</v>
-      </c>
-      <c r="G19">
+      <c r="O35" s="5">
+        <v>303</v>
+      </c>
+      <c r="P35" s="5">
+        <v>310</v>
+      </c>
+      <c r="Q35" s="21">
         <v>309</v>
       </c>
-      <c r="H19" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="R35">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="11" t="s">
+    </row>
+    <row r="36" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E36" s="38">
+        <v>182</v>
+      </c>
+      <c r="L36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="11">
-        <v>150</v>
-      </c>
-      <c r="E20">
-        <v>150</v>
-      </c>
-      <c r="F20" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>310</v>
-      </c>
-      <c r="H20" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>4</v>
-      </c>
-      <c r="J20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="M36" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="11">
+      <c r="N36" s="21">
         <v>77</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>-77</v>
-      </c>
-      <c r="G21">
+      <c r="O36" s="21">
         <v>303</v>
       </c>
-      <c r="H21" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="P36" s="21">
+        <v>311</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>306</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="J21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="11">
-        <v>77</v>
-      </c>
-      <c r="E22">
-        <v>77</v>
-      </c>
-      <c r="F22" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>311</v>
-      </c>
-      <c r="H22" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
+      <c r="S36">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="11">
-        <v>77</v>
-      </c>
-      <c r="E23">
-        <v>87</v>
-      </c>
-      <c r="F23" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>306</v>
-      </c>
-      <c r="H23" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="11">
-        <v>172</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>-172</v>
-      </c>
-      <c r="G24">
-        <v>312</v>
-      </c>
-      <c r="H24" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="11">
-        <v>172</v>
-      </c>
-      <c r="E25">
-        <v>172</v>
-      </c>
-      <c r="F25" s="17">
-        <f>Table2[[#This Row],[dump gen]]-Table2[[#This Row],[generation square is reached]]</f>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>304</v>
-      </c>
-      <c r="H25" s="17">
-        <f>Table2[[#This Row],[gens to reach]]-$G$3</f>
-        <v>-2</v>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E37" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0</v>
+      </c>
+      <c r="O37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="P37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="R37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="S37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="T37" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E38" s="38">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E39" s="37">
+        <v>80100</v>
+      </c>
+    </row>
+    <row r="40" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E40" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E41" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E42" s="38">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E43" s="38" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A115CE5B-AF13-48B8-8502-44F0B5743538}">
+  <dimension ref="B2:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>